<commit_message>
More stories and Competency Questions
</commit_message>
<xml_diff>
--- a/StoryBreakdown_Franzi.xlsx
+++ b/StoryBreakdown_Franzi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="243">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -33,6 +33,15 @@
     <t xml:space="preserve">A_Girl_Who_Lived_In_A_Cave_COW2</t>
   </si>
   <si>
+    <t xml:space="preserve">Milk_Bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children_of_Wax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brave_Hunter</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATU Class</t>
   </si>
   <si>
@@ -42,6 +51,9 @@
     <t xml:space="preserve"> 850-999 REALISTIC TALES</t>
   </si>
   <si>
+    <t xml:space="preserve">400-459: Supernatural or Enchanted Wife (Husband) or Other Relative</t>
+  </si>
+  <si>
     <t xml:space="preserve">Origin</t>
   </si>
   <si>
@@ -57,6 +69,15 @@
     <t xml:space="preserve">AGW</t>
   </si>
   <si>
+    <t xml:space="preserve">MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Squence</t>
   </si>
   <si>
@@ -66,6 +87,18 @@
     <t xml:space="preserve">βγδε1ζ1η3θA17B7HI5K10↓</t>
   </si>
   <si>
+    <t xml:space="preserve">βεζ3a2C↑HIK↓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">γδaCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">βε2ζ2η3λHI↓</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">Iβ. Absentation</t>
   </si>
   <si>
@@ -75,6 +108,12 @@
     <t xml:space="preserve">The girl could not believe that the family would be leaving the place where they had lived for so long […]</t>
   </si>
   <si>
+    <t xml:space="preserve">A man who had two clever children – a boy and a girl – ised tp gp tp a üöace wjere je lmew tjere were succulent wid fruits to be picked. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For this reason, he announced to all his friends that at the ceremony he would take the life of a leopard cub, as a sacrifice for the future of his young son.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iβ1. Absention of elders</t>
   </si>
   <si>
@@ -87,6 +126,9 @@
     <t xml:space="preserve">Iiy. Interdiction</t>
   </si>
   <si>
+    <t xml:space="preserve">The other children screamed, and some of them tried o grab at him as he left the hut, […]</t>
+  </si>
+  <si>
     <t xml:space="preserve">IIy1. Interdiction</t>
   </si>
   <si>
@@ -99,6 +141,9 @@
     <t xml:space="preserve">IIIδ. Violation</t>
   </si>
   <si>
+    <t xml:space="preserve">[…] but they failed to stop their brother and he was gone. </t>
+  </si>
+  <si>
     <t xml:space="preserve">IIIδ1. Interdiction Violated</t>
   </si>
   <si>
@@ -111,6 +156,9 @@
     <t xml:space="preserve">Ivε. Reconnaissance</t>
   </si>
   <si>
+    <t xml:space="preserve">At the end of the month, the children began to  be inquisitive about the source of the milk. </t>
+  </si>
+  <si>
     <t xml:space="preserve">IVε1. Reconnaissance by the villain to obtain information about the hero</t>
   </si>
   <si>
@@ -120,6 +168,9 @@
     <t xml:space="preserve">IVε2. Reconnaissance by the hero to obtain information about the villain</t>
   </si>
   <si>
+    <t xml:space="preserve">She searched through the forest for them, looking under all the trees and bushes and into all the secret forest places which leopards like to lie in. </t>
+  </si>
+  <si>
     <t xml:space="preserve">IVε3. Reconnaissance by other persons</t>
   </si>
   <si>
@@ -135,9 +186,15 @@
     <t xml:space="preserve">Vζ2. Hero receives information about the villain</t>
   </si>
   <si>
+    <t xml:space="preserve">When she saw the tracks that the hunter had made as he left the forest, she knew in her heart that a terrible thing had happened to her children […]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vζ3. Information received by other means</t>
   </si>
   <si>
+    <t xml:space="preserve">In this way they would know where the milk came from and their curiosity would be satisfied. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Viη. Trickery</t>
   </si>
   <si>
@@ -153,6 +210,9 @@
     <t xml:space="preserve">Then, when the stones where red hot, he put them in his mouth and let them lie against that part of his throat that made the sound. […] The stones had done what he had hope they would do and his voice was now as soft as the boy’s- </t>
   </si>
   <si>
+    <t xml:space="preserve">By the time she reached the hunter’s house she was one of the most beautiful women who had ever walked past that place.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VIIθ. Complicity</t>
   </si>
   <si>
@@ -168,6 +228,9 @@
     <t xml:space="preserve">“I am coming my brother,” the girl sang out. “The rock will move back and let you in.” </t>
   </si>
   <si>
+    <t xml:space="preserve">These words pleased the hunter, who shouted out to her that she could spend that night in his hut.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VIIIA. Villainy</t>
   </si>
   <si>
@@ -216,7 +279,7 @@
     <t xml:space="preserve">VIIIA13. Villain orders someone to be murdered</t>
   </si>
   <si>
-    <t xml:space="preserve">VIIIA14. Villain orders someone to be murdered</t>
+    <t xml:space="preserve">VIIIA14. Villain murders someone</t>
   </si>
   <si>
     <t xml:space="preserve">VIIIA15. Villain imprisons or detains someone</t>
@@ -246,6 +309,9 @@
     <t xml:space="preserve">VIIIa. Lack</t>
   </si>
   <si>
+    <t xml:space="preserve">The sun burned down on Ngwabi and before he had taken more than a few steps he felt all the strength drain from his limbs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VIIIa1. Lack of bride</t>
   </si>
   <si>
@@ -282,7 +348,7 @@
     <t xml:space="preserve">IXB5. Banished hero transported away from home</t>
   </si>
   <si>
-    <t xml:space="preserve">IXB6. Banished hero transported away from home</t>
+    <t xml:space="preserve">IXB6. Hero is condemned to death but secretly freed</t>
   </si>
   <si>
     <t xml:space="preserve">IXB7. A lament is sung</t>
@@ -297,12 +363,21 @@
     <t xml:space="preserve">He was not going to have his mother insulted in this way</t>
   </si>
   <si>
-    <t xml:space="preserve">XI. Departure</t>
+    <t xml:space="preserve">The boy was frightened of telling his father what had happened, and so he went out into the hills to look for another bird which was exactly the same as the bird which had escaped. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When night came, the children left their hut and went to the spot where Ngwabi had fallen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">XI. ↑ Departure</t>
   </si>
   <si>
     <t xml:space="preserve">[…] and the following day he arose early and flew to the highest tree that overlooked the fields of the new wife. </t>
   </si>
   <si>
+    <t xml:space="preserve">He searched in all the places he knew birds liked, but in none of these did he find a bird which looked at all similar. </t>
+  </si>
+  <si>
     <t xml:space="preserve">XIID. The first function of the donor</t>
   </si>
   <si>
@@ -432,6 +507,12 @@
     <t xml:space="preserve">When he saw the cannibal bending over his fire, the boy rushed forward and pushed him into the flames. </t>
   </si>
   <si>
+    <t xml:space="preserve">They seized two large sticks which were nearby […] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">He tried to rise to his feet, but he was not quick enough. </t>
+  </si>
+  <si>
     <t xml:space="preserve">XVIH1. They fight in an open field</t>
   </si>
   <si>
@@ -456,6 +537,12 @@
     <t xml:space="preserve">XVIII I. Victory</t>
   </si>
   <si>
+    <t xml:space="preserve">[…] drove the other boys away […]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before he could reach for his spear, the leopard mother was upon him. </t>
+  </si>
+  <si>
     <t xml:space="preserve">XVIII I1. The villain is beaten in open combat</t>
   </si>
   <si>
@@ -489,6 +576,12 @@
     <t xml:space="preserve">As they fell, from out of the wounds came the guinea fowl and his friends, crackling with joy at their freedom. </t>
   </si>
   <si>
+    <t xml:space="preserve">At once they knew it was the milk bird. Gently, the boy lifted up the milk bird […]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then, as the sun itself rose over the fields, the great bird which they had made suddenly moved its wings and launched itself into the air. </t>
+  </si>
+  <si>
     <t xml:space="preserve">XIXK1. Object is seized by force or cleverness</t>
   </si>
   <si>
@@ -525,10 +618,16 @@
     <t xml:space="preserve">XIXK11. Object received the same was as magical agent (See F)</t>
   </si>
   <si>
-    <t xml:space="preserve">XX. Return</t>
+    <t xml:space="preserve">XX. ↓  Return</t>
   </si>
   <si>
     <t xml:space="preserve">Soon they were back in the field, eating the last of the grain that was left. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[…] and carried it home. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The could not see, of course, the leopard mother playing with her cubs in the forest nor hear them singing their leopard songs in the darkness. </t>
   </si>
   <si>
     <t xml:space="preserve">XXIPr. Pursuit, chase</t>
@@ -685,16 +784,47 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC9900"/>
+        <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -743,12 +873,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -756,11 +934,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,7 +951,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF0066"/>
       <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -793,7 +967,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -819,7 +993,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFCC9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -841,1008 +1015,1663 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:G179"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9132653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.3673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0"/>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="0"/>
+      <c r="C14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="0"/>
+      <c r="C17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>31</v>
+      <c r="A18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="0"/>
+      <c r="C21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>36</v>
+      <c r="A22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="A23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>42</v>
+      <c r="A27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="0"/>
+      <c r="C27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>43</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="A30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>47</v>
+      <c r="A31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="0"/>
+      <c r="C31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>49</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="A33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="A34" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A35" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="A36" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="A37" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="A38" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="A39" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="A40" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="A41" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="A42" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A43" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="A44" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="A45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="A46" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="A47" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="A48" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="A49" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="A50" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="0"/>
+      <c r="C51" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A52" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="A53" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="A54" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
+      <c r="D54" s="0"/>
+      <c r="E54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>73</v>
+        <v>94</v>
+      </c>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+      <c r="D55" s="0"/>
+      <c r="E55" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="A56" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="A57" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="A58" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="A59" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
+      <c r="E59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="A60" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
+      <c r="D60" s="0"/>
+      <c r="E60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="A61" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
+      <c r="D61" s="0"/>
+      <c r="E61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>80</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
+      <c r="D62" s="0"/>
+      <c r="E62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="A63" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0"/>
+      <c r="E63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="A64" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="A65" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+      <c r="D65" s="0"/>
+      <c r="E65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="A66" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="A67" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="0"/>
+      <c r="C67" s="0"/>
+      <c r="D67" s="0"/>
+      <c r="E67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="A68" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="0"/>
+      <c r="C68" s="0"/>
+      <c r="D68" s="0"/>
+      <c r="E68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>88</v>
-      </c>
+      <c r="A69" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="0"/>
+      <c r="C69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="0"/>
+      <c r="E69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>90</v>
+        <v>111</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="0"/>
+      <c r="D70" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>92</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="0"/>
+      <c r="D71" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>93</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B72" s="0"/>
+      <c r="C72" s="0"/>
+      <c r="D72" s="0"/>
+      <c r="E72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="A73" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="0"/>
+      <c r="C73" s="0"/>
+      <c r="D73" s="0"/>
+      <c r="E73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="A74" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
+      <c r="D74" s="0"/>
+      <c r="E74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A75" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
+      <c r="D75" s="0"/>
+      <c r="E75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="A76" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
+      <c r="D76" s="0"/>
+      <c r="E76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="A77" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="0"/>
+      <c r="C77" s="0"/>
+      <c r="D77" s="0"/>
+      <c r="E77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="A78" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
+      <c r="D78" s="0"/>
+      <c r="E78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="A79" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
+      <c r="D79" s="0"/>
+      <c r="E79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="A80" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0"/>
+      <c r="D80" s="0"/>
+      <c r="E80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="A81" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" s="0"/>
+      <c r="C81" s="0"/>
+      <c r="D81" s="0"/>
+      <c r="E81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="A82" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
+      <c r="D82" s="0"/>
+      <c r="E82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="A83" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B83" s="0"/>
+      <c r="C83" s="0"/>
+      <c r="D83" s="0"/>
+      <c r="E83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>105</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B84" s="0"/>
+      <c r="C84" s="0"/>
+      <c r="D84" s="0"/>
+      <c r="E84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="A85" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="0"/>
+      <c r="C85" s="0"/>
+      <c r="D85" s="0"/>
+      <c r="E85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
-        <v>107</v>
-      </c>
+      <c r="A86" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
+      <c r="D86" s="0"/>
+      <c r="E86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="A87" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B87" s="0"/>
+      <c r="C87" s="0"/>
+      <c r="D87" s="0"/>
+      <c r="E87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="A88" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" s="0"/>
+      <c r="C88" s="0"/>
+      <c r="D88" s="0"/>
+      <c r="E88" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="A89" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" s="0"/>
+      <c r="C89" s="0"/>
+      <c r="D89" s="0"/>
+      <c r="E89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="A90" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
+      <c r="D90" s="0"/>
+      <c r="E90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="A91" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B91" s="0"/>
+      <c r="C91" s="0"/>
+      <c r="D91" s="0"/>
+      <c r="E91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="A92" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="0"/>
+      <c r="C92" s="0"/>
+      <c r="D92" s="0"/>
+      <c r="E92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="A93" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="0"/>
+      <c r="C93" s="0"/>
+      <c r="D93" s="0"/>
+      <c r="E93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="A94" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B94" s="0"/>
+      <c r="C94" s="0"/>
+      <c r="D94" s="0"/>
+      <c r="E94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>116</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B95" s="0"/>
+      <c r="C95" s="0"/>
+      <c r="D95" s="0"/>
+      <c r="E95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="A96" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
+      <c r="D96" s="0"/>
+      <c r="E96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="A97" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B97" s="0"/>
+      <c r="C97" s="0"/>
+      <c r="D97" s="0"/>
+      <c r="E97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="A98" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
+      <c r="D98" s="0"/>
+      <c r="E98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="A99" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
+      <c r="D99" s="0"/>
+      <c r="E99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
-        <v>121</v>
-      </c>
+      <c r="A100" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="0"/>
+      <c r="C100" s="0"/>
+      <c r="D100" s="0"/>
+      <c r="E100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="A101" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="0"/>
+      <c r="C101" s="0"/>
+      <c r="D101" s="0"/>
+      <c r="E101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="A102" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B102" s="0"/>
+      <c r="C102" s="0"/>
+      <c r="D102" s="0"/>
+      <c r="E102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A103" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B103" s="0"/>
+      <c r="C103" s="0"/>
+      <c r="D103" s="0"/>
+      <c r="E103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="A104" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B104" s="0"/>
+      <c r="C104" s="0"/>
+      <c r="D104" s="0"/>
+      <c r="E104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>126</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="B105" s="0"/>
+      <c r="C105" s="0"/>
+      <c r="D105" s="0"/>
+      <c r="E105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="A106" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B106" s="0"/>
+      <c r="C106" s="0"/>
+      <c r="D106" s="0"/>
+      <c r="E106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="A107" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B107" s="0"/>
+      <c r="C107" s="0"/>
+      <c r="D107" s="0"/>
+      <c r="E107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="A108" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B108" s="0"/>
+      <c r="C108" s="0"/>
+      <c r="D108" s="0"/>
+      <c r="E108" s="0"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="A109" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B109" s="0"/>
+      <c r="C109" s="0"/>
+      <c r="D109" s="0"/>
+      <c r="E109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="A110" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B110" s="0"/>
+      <c r="C110" s="0"/>
+      <c r="D110" s="0"/>
+      <c r="E110" s="0"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A111" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B111" s="0"/>
+      <c r="C111" s="0"/>
+      <c r="D111" s="0"/>
+      <c r="E111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B112" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>135</v>
+        <v>158</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E112" s="0"/>
+      <c r="F112" s="5" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="A113" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B113" s="0"/>
+      <c r="C113" s="0"/>
+      <c r="D113" s="0"/>
+      <c r="E113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2" t="s">
-        <v>137</v>
-      </c>
+      <c r="A114" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" s="0"/>
+      <c r="C114" s="0"/>
+      <c r="D114" s="0"/>
+      <c r="E114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="A115" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B115" s="0"/>
+      <c r="C115" s="0"/>
+      <c r="D115" s="0"/>
+      <c r="E115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A116" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B116" s="0"/>
+      <c r="C116" s="0"/>
+      <c r="D116" s="0"/>
+      <c r="E116" s="0"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>140</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B117" s="0"/>
+      <c r="C117" s="0"/>
+      <c r="D117" s="0"/>
+      <c r="E117" s="0"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="A118" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" s="0"/>
+      <c r="C118" s="0"/>
+      <c r="D118" s="0"/>
+      <c r="E118" s="0"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="A119" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B119" s="0"/>
+      <c r="C119" s="0"/>
+      <c r="D119" s="0"/>
+      <c r="E119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>143</v>
+        <v>170</v>
+      </c>
+      <c r="B120" s="0"/>
+      <c r="C120" s="0"/>
+      <c r="D120" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E120" s="0"/>
+      <c r="F120" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="A121" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B121" s="0"/>
+      <c r="C121" s="0"/>
+      <c r="D121" s="0"/>
+      <c r="E121" s="0"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="A122" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B122" s="0"/>
+      <c r="C122" s="0"/>
+      <c r="D122" s="0"/>
+      <c r="E122" s="0"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="A123" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B123" s="0"/>
+      <c r="C123" s="0"/>
+      <c r="D123" s="0"/>
+      <c r="E123" s="0"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="A124" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B124" s="0"/>
+      <c r="C124" s="0"/>
+      <c r="D124" s="0"/>
+      <c r="E124" s="0"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="s">
-        <v>148</v>
-      </c>
+      <c r="A125" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B125" s="0"/>
+      <c r="C125" s="0"/>
+      <c r="D125" s="0"/>
+      <c r="E125" s="0"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="A126" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D126" s="0"/>
+      <c r="E126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="A127" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B127" s="0"/>
+      <c r="C127" s="0"/>
+      <c r="D127" s="0"/>
+      <c r="E127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>154</v>
+        <v>182</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C128" s="0"/>
+      <c r="D128" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2" t="s">
-        <v>155</v>
-      </c>
+      <c r="A129" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B129" s="0"/>
+      <c r="C129" s="0"/>
+      <c r="D129" s="0"/>
+      <c r="E129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="A130" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B130" s="0"/>
+      <c r="C130" s="0"/>
+      <c r="D130" s="0"/>
+      <c r="E130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2" t="s">
-        <v>157</v>
-      </c>
+      <c r="A131" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B131" s="0"/>
+      <c r="C131" s="0"/>
+      <c r="D131" s="0"/>
+      <c r="E131" s="0"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="A132" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B132" s="0"/>
+      <c r="C132" s="0"/>
+      <c r="D132" s="0"/>
+      <c r="E132" s="0"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="A133" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B133" s="0"/>
+      <c r="C133" s="0"/>
+      <c r="D133" s="0"/>
+      <c r="E133" s="0"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="A134" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B134" s="0"/>
+      <c r="C134" s="0"/>
+      <c r="D134" s="0"/>
+      <c r="E134" s="0"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="A135" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B135" s="0"/>
+      <c r="C135" s="0"/>
+      <c r="D135" s="0"/>
+      <c r="E135" s="0"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A136" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B136" s="0"/>
+      <c r="C136" s="0"/>
+      <c r="D136" s="0"/>
+      <c r="E136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2" t="s">
-        <v>163</v>
-      </c>
+      <c r="A137" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B137" s="0"/>
+      <c r="C137" s="0"/>
+      <c r="D137" s="0"/>
+      <c r="E137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C138" s="0" t="s">
-        <v>165</v>
-      </c>
+      <c r="A138" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B138" s="0"/>
+      <c r="C138" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D138" s="0"/>
+      <c r="E138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A139" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B139" s="0"/>
+      <c r="C139" s="0"/>
+      <c r="D139" s="0"/>
+      <c r="E139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B140" s="0" t="s">
-        <v>168</v>
+        <v>198</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C140" s="0"/>
+      <c r="D140" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E140" s="12"/>
+      <c r="F140" s="5" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>170</v>
+      <c r="A141" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B141" s="0"/>
+      <c r="C141" s="6" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="A142" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="2" t="s">
-        <v>172</v>
-      </c>
+      <c r="A143" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B143" s="0"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="A144" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B144" s="0"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2" t="s">
-        <v>174</v>
-      </c>
+      <c r="A145" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="A146" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B146" s="0"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="A147" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B147" s="0"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="2" t="s">
-        <v>177</v>
-      </c>
+      <c r="A148" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B148" s="0"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>178</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="B149" s="0"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="2" t="s">
-        <v>179</v>
-      </c>
+      <c r="A150" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B150" s="0"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="A151" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B151" s="0"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2" t="s">
-        <v>181</v>
-      </c>
+      <c r="A152" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B152" s="0"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="2" t="s">
-        <v>182</v>
-      </c>
+      <c r="A153" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B153" s="0"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="A154" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B154" s="0"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2" t="s">
-        <v>184</v>
-      </c>
+      <c r="A155" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B155" s="0"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="A156" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B156" s="0"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2" t="s">
-        <v>186</v>
-      </c>
+      <c r="A157" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B157" s="0"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2" t="s">
-        <v>187</v>
-      </c>
+      <c r="A158" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B158" s="0"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2" t="s">
-        <v>188</v>
-      </c>
+      <c r="A159" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B159" s="0"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>189</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="B160" s="0"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>190</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B161" s="0"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>191</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>192</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="B163" s="0"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>193</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B164" s="0"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>194</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B165" s="0"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>195</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B166" s="0"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2" t="s">
-        <v>196</v>
-      </c>
+      <c r="A167" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B167" s="0"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="2" t="s">
-        <v>197</v>
-      </c>
+      <c r="A168" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B168" s="0"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2" t="s">
-        <v>198</v>
-      </c>
+      <c r="A169" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B169" s="0"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2" t="s">
-        <v>199</v>
-      </c>
+      <c r="A170" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B170" s="0"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>200</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="B171" s="0"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2" t="s">
-        <v>201</v>
-      </c>
+      <c r="A172" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="0"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B173" s="0" t="s">
-        <v>203</v>
+        <v>235</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2" t="s">
-        <v>204</v>
+      <c r="A174" s="11" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2" t="s">
-        <v>205</v>
+      <c r="A175" s="11" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="2" t="s">
-        <v>206</v>
+      <c r="A176" s="11" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="s">
-        <v>207</v>
+      <c r="A177" s="11" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="s">
-        <v>208</v>
+      <c r="A178" s="11" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2" t="s">
-        <v>209</v>
+      <c r="A179" s="11" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +2698,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1897,7 +2726,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>